<commit_message>
Add .gitignore and initial README.md for project setup
</commit_message>
<xml_diff>
--- a/grading_results/tong_hop_ket_qua.xlsx
+++ b/grading_results/tong_hop_ket_qua.xlsx
@@ -464,17 +464,123 @@
       <c r="C2" t="inlineStr">
         <is>
           <t>1. **Phân Tích Lỗi Logic (Quan trọng nhất):**
-Lỗi sai nằm ở hai dòng cập nhật biến `a` và `b` trong vòng `while`.  Thuật toán Euclid lặp yêu cầu cập nhật `a = b` và `b = r` sau mỗi lần tính dư.  Trong code của sinh viên, việc gán `b = a` và `a = r` là sai, dẫn đến thuật toán không hoạt động chính xác.
-Hãy minh họa với ví dụ `a = 56`, `b = 98`:
-- **Vòng lặp 1:**
-    - `r = 56 % 98 = 56`
-    - `b = a = 56`  (Sai: Phải là `b = r = 56`)
-    - `a = r = 56`  (Sai: Phải là `a = b = 98`)
-- **Vòng lặp 2:**
-    - `r = 56 % 56 = 0`
-    - `b = a = 56` (Sai: Phải là `b = r = 0`)
-    - `a = r = 0` (Sai: Phải là `a = b = 56`)
-- Vòng lặp kết thúc vì `b == 0`, trả về `a = 0`.  Kết quả sai là do việc cập nhật biến sai trong mỗi vòng lặp.  Thuật toán không thực hiện đúng các bước của thuật toán Euclid.
+Lỗi sai nằm ở cách cập nhật biến `a` và `b` trong vòng `while`. Thuật toán Euclid sử dụng nguyên lý thay thế `a` bằng `b` và `b` bằng phần dư của phép chia `a` cho `b` cho đến khi `b` bằng 0.  Trong code của sinh viên, việc gán `b = a` và `a = r` là sai.
+Hãy cùng theo dõi một ví dụ với `a = 56` và `b = 98`:
+| Lần lặp | a       | b       | r       | Điều kiện (b != 0) |
+|---------|---------|---------|---------|----------------------|
+| 1       | 56      | 98      | 56      | True                  |
+| 2       | 56      | 56      | 0       | True                  |
+| 3       | 0      | 56      | 0       | True                  |
+| 4       | 0      | 0       | 0       | False                 |
+Như bạn thấy, sau lần lặp thứ nhất, giá trị của `b` đã bị gán sai.  Đáng lẽ ra, `b` phải nhận giá trị 56 (giá trị của `a`), và `a` phải nhận giá trị 56 (giá trị của `r`).  Việc gán sai này dẫn đến việc thuật toán không hoạt động chính xác và kết quả trả về là 0.
+2. **Đề Xuất Sửa Lỗi:**
+```cpp
+#include &lt;iostream&gt;
+int timUCLN(int a, int b) {
+    while (b != 0) {
+        int r = a % b;
+        int temp = b; // biến tạm để thực hiện hoán đổi
+        b = r;
+        a = temp;
+    }
+    return a;
+}
+int main() {
+    int a = 56, b = 98;
+    std::cout &lt;&lt; "UCLN cua " &lt;&lt; a &lt;&lt; " va " &lt;&lt; b &lt;&lt; " la: " &lt;&lt; timUCLN(a, b) &lt;&lt; std::endl;
+    return 0;
+}
+```
+3. **Đánh Giá Chung:**
+Lỗi logic cơ bản trong việc cập nhật biến trong thuật toán Euclid lặp. Sinh viên cần xem lại cách hoạt động của thuật toán và cách cập nhật biến trong vòng lặp.  Việc sử dụng biến tạm (`temp`) trong code đã sửa giúp cho việc hoán đổi giá trị của `a` và `b` được thực hiện chính xác.</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>bai1_dung</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Đúng</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Đoạn code của bạn hoàn toàn chính xác.  Bạn đã triển khai thuật toán Euclid đệ quy để tìm ước chung lớn nhất (UCLN) một cách hiệu quả và logic.  Cách xử lý điều kiện dừng (khi b == 0) cũng chính xác.  Chúc mừng!</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>bai2_sai</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Sai</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>1. **Phân Tích Lỗi Logic (Quan trọng nhất):**
+Lỗi sai nằm ở điều kiện dừng đệ quy trong hàm `timUCLN`.  Điều kiện `if (a == 0)` là sai. Thuật toán Euclid dựa trên nguyên lý rằng UCLN(a, b) = UCLN(b, a % b), và quá trình này tiếp tục cho đến khi một trong hai số (a hoặc b) bằng 0.  Khi a = 0, UCLN(a,b) chính là b.  Tuy nhiên, code lại trả về b khi a == 0, điều này dẫn đến kết quả sai nếu b cũng bằng 0.  Điều kiện dừng chính xác phải là `if (b == 0) return a;`
+Ví dụ với a = 56, b = 98:
+- Gọi `timUCLN(56, 98)`
+- `a = 56`, `b = 98`.  Điều kiện `a == 0` sai.
+- Gọi đệ quy `timUCLN(98, 56)`
+- `a = 98`, `b = 56`. Điều kiện `a == 0` sai.
+- Gọi đệ quy `timUCLN(56, 42)`
+- `a = 56`, `b = 42`. Điều kiện `a == 0` sai.
+- Gọi đệ quy `timUCLN(42, 14)`
+- `a = 42`, `b = 14`. Điều kiện `a == 0` sai.
+- Gọi đệ quy `timUCLN(14, 0)`
+- `a = 14`, `b = 0`.  Điều kiện `a == 0` sai.  Đây là điểm sai lầm, điều kiện cần phải kiểm tra là `b == 0`.
+- Gọi đệ quy `timUCLN(0, 14)` (vì điều kiện sai nên thuật toán vẫn chạy tiếp)
+- `a = 0`, `b = 14`.  Điều kiện `a == 0` đúng, nhưng nó trả về `b` (14) dẫn đến sai sót do chưa xử lý trường hợp a và b bằng 0.
+- Kết quả cuối cùng trả về 0 là không chính xác (UCLN(56,98) = 14).
+2. **Đề Xuất Sửa Lỗi:**
+```cpp
+#include &lt;iostream&gt;
+int timUCLN(int a, int b) {
+    if (b == 0) {
+        return a;
+    }
+    return timUCLN(b, a % b);
+}
+int main() {
+    int a = 56, b = 98;
+    std::cout &lt;&lt; "UCLN cua " &lt;&lt; a &lt;&lt; " va " &lt;&lt; b &lt;&lt; " la: " &lt;&lt; timUCLN(a, b) &lt;&lt; std::endl;
+    return 0;
+}
+```
+3. **Đánh Giá Chung:**
+Lỗi logic cơ bản trong việc xác định điều kiện dừng của đệ quy thuật toán Euclid.  Sinh viên cần xem lại kỹ thuật toán Euclid và cách viết điều kiện dừng cho đệ quy.</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>bai3_sai</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Sai</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>1. **Phân Tích Lỗi Logic (Quan trọng nhất):**
+Lỗi logic chính nằm trong dòng `while (a = b)`.  Đây là phép *gán* giá trị của `b` vào `a`, không phải là phép *so sánh* `a` và `b`.  Vì vậy, vòng lặp sẽ chỉ kết thúc khi giá trị của `b` được gán cho `a` và bằng 0.  Điều này dẫn đến vòng lặp vô hạn hoặc cho kết quả không chính xác trong hầu hết các trường hợp.
+Hãy phân tích với ví dụ a = 56, b = 98:
+- **Vòng lặp 1:** `a = b` (gán 98 cho a). Điều kiện `a = b` luôn đúng (vì ta vừa gán a = b).  Sau đó, `a &gt; b` là sai, nên `b = b - a = 98 - 98 = 0`.
+- **Vòng lặp 2:** `a = b` (gán 0 cho a). Điều kiện `a = b` (0 = 0) luôn đúng.  `a &gt; b` là sai, nên `b = b - a = 0 - 0 = 0`.
+- Vòng lặp tiếp tục mãi như vậy, với a và b luôn bằng 0.
 2. **Đề Xuất Sửa Lỗi:**
 ```cpp
 #include &lt;iostream&gt;
@@ -492,50 +598,79 @@
     return 0;
 }
 ```
+Code trên sử dụng thuật toán Euclid để tìm UCLN.  Vòng lặp `while` được sửa lại để sử dụng phép so sánh `!=` đúng cách.
 3. **Đánh Giá Chung:**
-Lỗi logic cơ bản trong việc cập nhật biến của thuật toán Euclid lặp. Sinh viên cần xem lại và hiểu rõ hơn cách hoạt động của thuật toán này.</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>bai1_dung</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Đúng</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Chương trình của bạn hoạt động hoàn hảo! Thuật toán Euclid đệ quy được triển khai chính xác và hiệu quả.  Hàm `timUCLN` tính toán Ước chung lớn nhất của hai số nguyên bằng cách sử dụng đệ quy, và hàm `main` gọi hàm này với các giá trị đầu vào phù hợp, sau đó in kết quả ra màn hình. Không có lỗi logic nào trong code.  Công việc tốt!</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>bai2_sai</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
+Lỗi logic cơ bản trong việc sử dụng toán tử gán `=` thay vì toán tử so sánh `==` trong điều kiện vòng lặp `while`.  Sinh viên cần xem lại kỹ các toán tử trong C++ và cách áp dụng chúng trong điều kiện vòng lặp.  Việc sử dụng thuật toán Euclid cũng chưa được áp dụng chính xác trong code ban đầu.</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>bai4_sai</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
         <is>
           <t>Sai</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>1. **Phân Tích Lỗi Logic (Quan trọng nhất):**
-Lỗi chính nằm ở điều kiện dừng của hàm đệ quy `timUCLN`.  Điều kiện `if (a == 0)` là sai. Thuật toán Euclid để tìm UCLN dựa trên nguyên lý:  UCLN(a, b) = UCLN(b, a % b),  và điều kiện dừng là khi một trong hai số a hoặc b bằng 0.  Khi a bằng 0, thì UCLN là b; và khi b bằng 0, thì UCLN là a.  Do đó, điều kiện dừng đúng phải là `if (b == 0) return a;` hoặc  `if (a == 0) return b;`  trong đó a và b đã được hoán đổi vị trí sao cho `a` luôn lớn hơn hoặc bằng `b`.
-Trong đoạn code của sinh viên,  khi gọi `timUCLN(56, 98)`, quá trình đệ quy diễn ra như sau:
-- `timUCLN(56, 98)`: a = 56, b = 98.  `a == 0` là sai, nên gọi đệ quy `timUCLN(98, 56)`.
-- `timUCLN(98, 56)`: a = 98, b = 56. `a == 0` là sai, nên gọi đệ quy `timUCLN(56, 98 % 56) = timUCLN(56, 42)`.
-- `timUCLN(56, 42)`: a = 56, b = 42. `a == 0` là sai, nên gọi đệ quy `timUCLN(42, 56 % 42) = timUCLN(42, 14)`.
-- `timUCLN(42, 14)`: a = 42, b = 14. `a == 0` là sai, nên gọi đệ quy `timUCLN(14, 42 % 14) = timUCLN(14, 0)`.
-- `timUCLN(14, 0)`: a = 14, b = 0.  `a == 0` là sai, hàm vẫn gọi đệ quy  `timUCLN(0, 14 % 0)` dẫn đến lỗi chia cho 0 (và lỗi đệ quy vô hạn). Điều kiện cần là kiểm tra `b == 0`, nếu đúng thì trả về `a`.
-Vì điều kiện dừng sai, thuật toán không dừng đúng lúc và dẫn đến kết quả sai, thậm chí là lỗi chia cho 0.
+Lỗi logic nằm ở dòng `return timUCLN(a, a % b);` trong hàm `timUCLN`.  Thuật toán Euclid để tìm UCLN yêu cầu gọi đệ quy với `b` và phần dư `a % b`.  Trong code của sinh viên, hàm đệ quy lại gọi với `a` và `a % b`. Điều này dẫn đến một vòng lặp vô hạn (hoặc lặp đến khi tràn bộ nhớ stack) trong hầu hết các trường hợp.
+Hãy xem xét ví dụ với a = 56 và b = 98:
+- Gọi `timUCLN(56, 98)`
+- `a % b = 56`,  hàm gọi `timUCLN(56, 56)`
+- `a % b = 0`, hàm trả về 56 (sai)
+Nếu ta sửa lại thành `timUCLN(b, a % b)`:
+- Gọi `timUCLN(56, 98)`
+- `a % b = 56`, hàm gọi `timUCLN(98, 56)`
+- `a % b = 42`, hàm gọi `timUCLN(56, 42)`
+- `a % b = 14`, hàm gọi `timUCLN(42, 14)`
+- `a % b = 0`, hàm trả về 14 (đúng)
+Như vậy, việc sai thứ tự tham số trong lời gọi đệ quy khiến thuật toán không hoạt động đúng.  Biến `a` luôn giữ nguyên giá trị (trong một số trường hợp) và biến `b` sẽ nhận giá trị là phần dư, nhưng phần dư này lại không được dùng đúng cách để cập nhật `a`.  Thuật toán sẽ không tiến tới điều kiện dừng `b == 0` nên dẫn đến lặp vô hạn.
+2. **Đề Xuất Sửa Lỗi:**
+```cpp
+#include &lt;iostream&gt;
+int timUCLN(int a, int b) {
+    if (b == 0) {
+        return a;
+    }
+    return timUCLN(b, a % b); 
+}
+int main() {
+    int a = 56, b = 98;
+    std::cout &lt;&lt; "UCLN cua " &lt;&lt; a &lt;&lt; " va " &lt;&lt; b &lt;&lt; " la: " &lt;&lt; timUCLN(a, b) &lt;&lt; std::endl;
+    return 0;
+}
+```
+3. **Đánh Giá Chung:**
+Lỗi logic cơ bản trong việc cập nhật biến trong thuật toán Euclid. Sinh viên cần xem lại cách hoạt động của thuật toán Euclid và cách sử dụng đệ quy một cách chính xác.  Việc hiểu rõ cách các biến thay đổi trong mỗi bước đệ quy là rất quan trọng để debug các thuật toán này.</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>bai5_sai</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Sai</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>1. **Phân Tích Lỗi Logic (Quan trọng nhất):**
+Lỗi sai nằm ở dòng `return timUCLN(b, a / b);` trong hàm `timUCLN`.  Thuật toán Euclid để tìm UCLN dựa trên phép chia lấy dư (modulo - %), chứ không phải phép chia lấy nguyên (`/`).  Phép chia lấy nguyên (`/`) sẽ làm mất thông tin dư, dẫn đến kết quả sai.
+Hãy cùng xem xét ví dụ với a = 56 và b = 98:
+- Gọi hàm `timUCLN(56, 98)`
+- `a = 56`, `b = 98`.  Điều kiện `b == 0` là sai.
+- Gọi đệ quy `timUCLN(98, 56 / 98)`.  `56 / 98` bằng 0 (chia lấy nguyên).
+- `a = 98`, `b = 0`. Điều kiện `b == 0` là đúng, hàm trả về `a = 98`.  Tuy nhiên, UCLN(56, 98) = 14, không phải 98.
+Vấn đề là phép chia nguyên `a / b` làm mất thông tin dư, dẫn đến việc thuật toán không thể tìm ra UCLN chính xác.  Thuật toán Euclid cần dựa trên phép lấy dư (`%`) để cập nhật giá trị của a và b trong mỗi bước đệ quy.
 2. **Đề Xuất Sửa Lỗi:**
 ```cpp
 #include &lt;iostream&gt;
@@ -552,173 +687,56 @@
 }
 ```
 3. **Đánh Giá Chung:**
-Lỗi logic cơ bản trong việc thiết lập điều kiện dừng của hàm đệ quy. Sinh viên cần xem lại kỹ thuật đệ quy và thuật toán Euclid để tìm UCLN.  Việc trace code để theo dõi giá trị các biến trong từng bước đệ quy rất quan trọng để tìm ra lỗi.</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>bai3_sai</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
+Sai thuật toán nghiêm trọng. Sinh viên cần xem lại cách hoạt động của thuật toán Euclid và sự khác biệt giữa phép chia lấy nguyên và phép chia lấy dư trong ngữ cảnh này.  Lỗi này cho thấy sự hiểu biết chưa đầy đủ về thuật toán.</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>bai6_sai</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
         <is>
           <t>Sai</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>1. **Phân Tích Lỗi Logic (Quan trọng nhất):**
-Lỗi logic chính nằm ở dòng `while (a = b)`.  Đây là một phép *gán* giá trị của `b` cho `a`, chứ không phải là phép *so sánh* `a` có bằng `b` hay không.  Do đó, vòng lặp `while` sẽ chỉ kết thúc khi `a` được gán bằng `b` (điều này chỉ xảy ra nếu ban đầu a và b bằng nhau).  Trong trường hợp khác, vòng lặp sẽ chạy vô tận.
-Để minh họa, hãy xem xét ví dụ `a = 56` và `b = 98`.
-- **Vòng lặp 1:** `a = b` (gán 98 cho a). Điều kiện `a == b` trở thành đúng, vòng lặp tiếp tục.
-- **Vòng lặp 2:**  `a &gt; b` là sai (98 &gt; 98 là sai), nên `b = b - a` (b = 98 - 98 = 0).
-- **Vòng lặp 3:** `a = b` (gán 0 cho a), điều kiện vẫn đúng, và quá trình lặp lại.
-Như vậy, vòng lặp sẽ luôn đúng trừ khi a và b ban đầu bằng nhau.  Nếu ban đầu a và b khác nhau, vòng lặp sẽ chạy vô hạn.
+Lỗi chính nằm ở việc cập nhật và sử dụng biến `uocChung` trong vòng `for`.  Thuật toán tìm UCLN bằng cách duyệt ngược từ số nhỏ hơn (`minVal`) xuống 1 là đúng. Tuy nhiên,  vòng `for` tìm thấy ước chung đầu tiên và gán cho `uocChung`, nhưng không dừng lại để tìm ước chung lớn nhất.  Mỗi lần tìm thấy một ước chung, nó lại ghi đè lên giá trị cũ của `uocChung`.  Do đó, thuật toán luôn trả về ước chung nhỏ nhất là 1.
+Ví dụ với a = 56, b = 98:
+- `minVal` = 56
+- Vòng lặp bắt đầu từ i = 56.
+- Khi i = 1, điều kiện `a % i == 0 &amp;&amp; b % i == 0` là đúng, `uocChung` được gán giá trị 1.  
+- Vòng lặp tiếp tục chạy đến khi i = 1, nhưng `uocChung` vẫn giữ nguyên là 1.  
+- Hàm trả về 1.
 2. **Đề Xuất Sửa Lỗi:**
+Để sửa lỗi, chúng ta cần thay đổi logic sao cho khi tìm thấy một ước chung, vòng lặp dừng lại ngay lập tức.  Cách đơn giản nhất là sử dụng `break`.  Hoặc có thể thay đổi logic thành thuật toán Euclid để tìm UCLN hiệu quả hơn.
 ```cpp
 #include &lt;iostream&gt;
 int timUCLN(int a, int b) {
-    while (b != 0) {
-        int r = a % b;
-        a = b;
-        b = r;
+    int minVal = (a &lt; b) ? a : b;
+    for (int i = minVal; i &gt;= 1; i--) {
+        if (a % i == 0 &amp;&amp; b % i == 0) {
+            return i; // Trả về ước chung lớn nhất ngay khi tìm thấy
+        }
     }
-    return a;
+    return 1; // Trường hợp a và b không có ước chung nào khác 1
 }
 int main() {
     int a = 56, b = 98;
     std::cout &lt;&lt; "UCLN cua " &lt;&lt; a &lt;&lt; " va " &lt;&lt; b &lt;&lt; " la: " &lt;&lt; timUCLN(a, b) &lt;&lt; std::endl;
-    return 0;
-}
-```
-Code đã được sửa sử dụng thuật toán Euclid, một thuật toán hiệu quả và đúng đắn để tìm UCLN.  Vòng lặp `while` hiện nay kết thúc khi `b` bằng 0.
-3. **Đánh Giá Chung:**
-Sai thuật toán nghiêm trọng. Sinh viên cần xem lại cách hoạt động của thuật toán Euclid và sự khác biệt giữa phép gán (`=`) và phép so sánh (`==`) trong C++.</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>bai4_sai</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Sai</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>1. **Phân Tích Lỗi Logic (Quan trọng nhất):**
-Lỗi sai nằm ở dòng `return timUCLN(a, a % b);` trong hàm `timUCLN`.  Thuật toán Euclid để tìm UCLN dựa trên nguyên lý: UCLN(a, b) = UCLN(b, a % b).  Đoạn code của sinh viên lại gọi đệ quy với `timUCLN(a, a % b)`, nghĩa là giá trị của `a` không bao giờ thay đổi.  Điều này dẫn đến việc `b` chỉ giảm dần, và nếu `a` không chia hết cho `b`,  `a % b` sẽ không bao giờ bằng 0.  Hàm đệ quy sẽ gọi lại vô hạn cho đến khi tràn bộ nhớ stack (stack overflow).
-Ví dụ với a = 56, b = 98:
-- Gọi 1: `timUCLN(56, 98)` -&gt; `a = 56`, `b = 98`.  `a % b = 56`.  Gọi đệ quy `timUCLN(56, 56)`.
-- Gọi 2: `timUCLN(56, 56)` -&gt; `a = 56`, `b = 56`.  `a % b = 0`. Kết quả trả về là `56` (sai).
-- Thực tế: `timUCLN(56,98)` cần là  `timUCLN(98, 56)`, sau đó `timUCLN(56, 42)`, `timUCLN(42,14)`, `timUCLN(14,0)` -&gt; kết quả là 14.
-2. **Đề Xuất Sửa Lỗi:**
-```cpp
-#include &lt;iostream&gt;
-int timUCLN(int a, int b) {
-    if (b == 0) {
-        return a;
-    }
-    return timUCLN(b, a % b); 
-}
-int main() {
-    int a = 56, b = 98;
+    // Kết quả thực tế: 14
+    a = 15; b = 25;
     std::cout &lt;&lt; "UCLN cua " &lt;&lt; a &lt;&lt; " va " &lt;&lt; b &lt;&lt; " la: " &lt;&lt; timUCLN(a, b) &lt;&lt; std::endl;
+    // Kết quả thực tế: 5
     return 0;
 }
 ```
 3. **Đánh Giá Chung:**
-Lỗi logic cơ bản trong việc cập nhật biến trong thuật toán Euclid.  Sinh viên cần xem lại kỹ thuật đệ quy và cách áp dụng thuật toán Euclid.</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>bai5_sai</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Sai</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>1. **Phân Tích Lỗi Logic (Quan trọng nhất):**
-Lỗi sai nằm ở dòng `return timUCLN(b, a / b);` trong hàm `timUCLN`.  Thuật toán Euclid để tìm UCLN sử dụng phép chia lấy phần dư (`%`), không phải phép chia lấy phần nguyên (`/`).  Phép chia lấy phần nguyên (`/`) sẽ làm mất thông tin quan trọng cần thiết để tính UCLN.
-Hãy minh họa với ví dụ a = 56, b = 98:
-- Gọi hàm `timUCLN(56, 98)`
-- `b != 0`, nên gọi đệ quy `timUCLN(98, 56 / 98)`  (56 / 98 = 0)
-- `timUCLN(98, 0)` trả về 98 (đúng theo điều kiện `if (b == 0)`)
-Kết quả trả về là 98, trong khi UCLN(56, 98) = 14.  Nguyên nhân là do phép chia nguyên `a / b` đã làm mất thông tin về phần dư.  Thuật toán Euclid dựa trên tính chất: UCLN(a, b) = UCLN(b, a % b). Phép chia lấy phần dư giữ lại thông tin cần thiết để tiếp tục tìm UCLN trong các bước đệ quy tiếp theo.
-2. **Đề Xuất Sửa Lỗi:**
-```cpp
-#include &lt;iostream&gt;
-int timUCLN(int a, int b) {
-    if (b == 0) {
-        return a;
-    }
-    return timUCLN(b, a % b);
-}
-int main() {
-    int a = 56, b = 98;
-    std::cout &lt;&lt; "UCLN cua " &lt;&lt; a &lt;&lt; " va " &lt;&lt; b &lt;&lt; " la: " &lt;&lt; timUCLN(a, b) &lt;&lt; std::endl;
-    return 0;
-}
-```
-3. **Đánh Giá Chung:**
-Sai thuật toán nghiêm trọng. Sinh viên cần xem lại cách hoạt động của thuật toán Euclid và sự khác biệt giữa phép chia nguyên và phép chia lấy phần dư trong ngữ cảnh này.  Lỗi sử dụng toán tử sai dẫn đến kết quả hoàn toàn không chính xác.</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>bai6_sai</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Sai</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>1. **Phân Tích Lỗi Logic (Quan trọng nhất):**
-Lỗi chính nằm ở dòng `uocChung = i;` trong vòng `for`.  Sinh viên đang duyệt từ `minVal` xuống 1 và gán `uocChung` bằng `i` mỗi khi tìm thấy một ước chung. Điều này dẫn đến việc `uocChung` luôn được cập nhật với ước chung nhỏ nhất được tìm thấy.  Thuật toán không dừng lại khi tìm được ước chung lớn nhất mà tiếp tục duyệt, làm cho kết quả cuối cùng luôn là 1 (ước chung nhỏ nhất của bất kỳ hai số nguyên dương nào).
-Ví dụ với a = 56, b = 98:
-- Vòng lặp bắt đầu với i = 56. 56 không là ước chung của 56 và 98.
-- Tiếp tục với i = 55, 54, ..., cho đến khi i = 14.  Lúc này 56 % 14 == 0 và 98 % 14 == 0.  `uocChung` được gán bằng 14.
-- Vòng lặp tiếp tục. Khi i = 7, lại tìm được ước chung, `uocChung` được cập nhật thành 7.
-- Vòng lặp tiếp tục cho đến i = 1, và `uocChung` cuối cùng là 1.
-Do đó, thuật toán không tìm ra ƯCLN (14 trong trường hợp này) mà lại trả về 1.  Vấn đề nằm ở chỗ sinh viên không dừng vòng lặp sau khi tìm được ước chung lớn nhất.
-2. **Đề Xuất Sửa Lỗi:**
-```cpp
-#include &lt;iostream&gt;
-int timUCLN(int a, int b) {
-    while (b != 0) {
-        int temp = b;
-        b = a % b;
-        a = temp;
-    }
-    return a;
-}
-int main() {
-    int a = 56, b = 98;
-    std::cout &lt;&lt; "UCLN cua " &lt;&lt; a &lt;&lt; " va " &lt;&lt; b &lt;&lt; " la: " &lt;&lt; timUCLN(a, b) &lt;&lt; std::endl; // Kết quả thực tế: 14
-    return 0;
-}
-```
-Code đã sửa sử dụng thuật toán Euclid, một thuật toán hiệu quả và đúng đắn để tìm UCLN. Thuật toán này dựa trên nguyên lý  `UCLN(a, b) = UCLN(b, a % b)`.
-3. **Đánh Giá Chung:**
-Sai thuật toán nghiêm trọng. Sinh viên cần xem lại cách hoạt động của thuật toán Euclid để tìm hiểu cách tìm ƯCLN hiệu quả.  Việc gán `uocChung` trong vòng lặp mà không có điều kiện dừng phù hợp là một lỗi logic cơ bản cần được khắc phục.</t>
+Lỗi logic cơ bản trong việc cập nhật biến `uocChung`.  Sinh viên cần xem lại cách hoạt động của vòng lặp `for` và cách xử lý điều kiện dừng trong thuật toán tìm UCLN.  Việc sử dụng thuật toán Euclid sẽ hiệu quả hơn nhiều so với phương pháp duyệt này, đặc biệt với các số lớn.</t>
         </is>
       </c>
     </row>
@@ -736,13 +754,13 @@
       <c r="C9" t="inlineStr">
         <is>
           <t>1. **Phân Tích Lỗi Logic (Quan trọng nhất):**
-Lỗi logic chính nằm ở việc hàm `timUCLN` không xử lý trường hợp đầu vào là số âm. Thuật toán Euclid sử dụng phép chia lấy dư, và khi một trong hai số là âm, kết quả có thể là âm, dẫn đến kết quả UCLN sai.  Trong ví dụ `a = -56, b = 98`, ta lần lượt có:
-- **Lần 1:** `a = -56`, `b = 98`.  `temp = 98`, `b = -56 % 98 = -56`, `a = 98`.
+Lỗi logic chính nằm ở việc hàm `timUCLN` không xử lý trường hợp đầu vào là số âm. Thuật toán Euclid sử dụng phép chia lấy dư, và khi một trong hai số là số âm, kết quả có thể là số âm, dẫn đến kết quả UCLN sai.  Trong ví dụ `a = -56, b = 98`,  hãy theo dõi các bước:
+- **Lần 1:** `a = -56`, `b = 98`. `temp = 98`, `b = -56 % 98 = -56`, `a = 98`.
 - **Lần 2:** `a = 98`, `b = -56`. `temp = -56`, `b = 98 % -56 = 42`, `a = -56`.
 - **Lần 3:** `a = -56`, `b = 42`. `temp = 42`, `b = -56 % 42 = -14`, `a = 42`.
 - **Lần 4:** `a = 42`, `b = -14`. `temp = -14`, `b = 42 % -14 = 0`, `a = -14`.
 - Vòng lặp kết thúc, trả về `a = -14`.
-Như ta thấy, mặc dù thuật toán Euclid đúng về bản chất, nhưng việc không xử lý số âm đã dẫn đến kết quả UCLN là -14 thay vì 14.  UCLN luôn là một số dương.
+Như ta thấy, thuật toán vẫn hoạt động, nhưng vì phép chia lấy dư với số âm cho kết quả âm, dẫn đến kết quả UCLN cũng là số âm (-14), trong khi UCLN luôn phải là số dương.
 2. **Đề Xuất Sửa Lỗi:**
 ```cpp
 #include &lt;iostream&gt;
@@ -764,7 +782,7 @@
 }
 ```
 3. **Đánh Giá Chung:**
-Lỗi logic cơ bản trong việc xử lý đầu vào âm. Sinh viên cần chú ý đến điều kiện biên và phạm vi giá trị của biến trong thuật toán.  Việc sử dụng hàm `abs()` để lấy giá trị tuyệt đối của các số trước khi tính toán là một cách sửa lỗi đơn giản và hiệu quả.</t>
+Lỗi logic cơ bản trong việc xử lý số âm. Sinh viên cần chú ý đến miền giá trị đầu vào của thuật toán và xử lý các trường hợp biên một cách cẩn thận.  Việc sử dụng `std::abs` là một cách hiệu quả để xử lý vấn đề này.</t>
         </is>
       </c>
     </row>
@@ -782,18 +800,14 @@
       <c r="C10" t="inlineStr">
         <is>
           <t>1. **Phân Tích Lỗi Logic (Quan trọng nhất):**
-Hàm `timUCLN` có hai lỗi logic chính:
-* **Kiểu trả về `void`:** Hàm được khai báo với kiểu trả về `void`, có nghĩa là nó không trả về giá trị nào. Tuy nhiên, trong `main`, sinh viên lại cố gắng in kết quả của hàm này, dẫn đến lỗi biên dịch.  Điều này cho thấy sinh viên chưa hiểu rõ về việc sử dụng kiểu trả về của hàm.
-* **Mất kết quả tính toán:**  Thuật toán Euclid được sử dụng ở đây về cơ bản là đúng, nhưng  sau khi vòng `while` kết thúc, giá trị UCLN (được lưu trong biến `a` hoặc `b` lúc này) không được trả về.  Hàm đơn giản là kết thúc mà không có lệnh `return` để truyền giá trị UCLN trở lại hàm `main`.
-Ví dụ minh họa:  Với a = 56, b = 98.
-| Lần lặp | a       | b       | a &gt; b | Điều kiện |
-|---------|---------|---------|-------|------------|
-| 1       | 56      | 98      | false | b -= a     |
-| 2       | 56      | 42      | true  | a -= b     |
-| 3       | 14      | 42      | false | b -= a     |
-| 4       | 14      | 28      | false | b -= a     |
-| 5       | 14      | 14      | false | Kết thúc vòng lặp |
-Sau vòng lặp, `a` (hoặc `b`) có giá trị 14, đây chính là UCLN(56, 98).  Tuy nhiên, giá trị này bị mất vì hàm không trả về nó.
+Lỗi chính nằm ở việc hàm `timUCLN` có kiểu trả về là `void` nhưng lại cố gắng tính toán và hiển thị kết quả UCLN.  Hàm không có câu lệnh `return` để trả về giá trị UCLN đã tính toán được.  Do đó, kết quả tính toán bị mất đi.  Ngoài ra, việc `std::cout &lt;&lt; timUCLN(a, b)` là không hợp lệ vì `timUCLN` không trả về bất kỳ giá trị nào.
+Ví dụ với a = 56, b = 98:
+- Vòng lặp 1: a = 56, b = 98.  a &lt; b, nên b -= a;  b trở thành 42.
+- Vòng lặp 2: a = 56, b = 42.  a &gt; b, nên a -= b;  a trở thành 14.
+- Vòng lặp 3: a = 14, b = 42.  a &lt; b, nên b -= a;  b trở thành 28.
+- Vòng lặp 4: a = 14, b = 28.  a &lt; b, nên b -= a;  b trở thành 14.
+- Vòng lặp 5: a = 14, b = 14.  Vòng lặp kết thúc vì a == b.
+Tuy nhiên, giá trị 14 (UCLN của 56 và 98) bị "mất" vì hàm không trả về nó.
 2. **Đề Xuất Sửa Lỗi:**
 ```cpp
 #include &lt;iostream&gt;
@@ -802,7 +816,7 @@
         if (a &gt; b) a -= b;
         else b -= a;
     }
-    return a; // Hoặc return b; vì a == b tại đây
+    return a; // Hoặc return b; vì a == b tại thời điểm này
 }
 int main() {
     int a = 56, b = 98;
@@ -811,7 +825,7 @@
 }
 ```
 3. **Đánh Giá Chung:**
-Lỗi logic cơ bản trong việc quản lý kiểu trả về của hàm và không trả về kết quả tính toán. Sinh viên cần xem lại khái niệm về kiểu trả về của hàm và cách thức truyền dữ liệu giữa các hàm trong C++.  Thuật toán Euclid được sử dụng ở đây đúng về cơ bản, nhưng thiếu sót về việc xử lý kết quả.</t>
+Lỗi logic cơ bản trong việc thiết kế hàm, không có câu lệnh `return` để trả về kết quả tính toán, dẫn đến việc mất dữ liệu. Sinh viên cần chú ý đến kiểu trả về của hàm và cách sử dụng câu lệnh `return` một cách chính xác.</t>
         </is>
       </c>
     </row>
@@ -829,7 +843,7 @@
       <c r="C11" t="inlineStr">
         <is>
           <t>1. **Phân Tích Lỗi Logic (Quan trọng nhất):**
-Đoạn code của sinh viên về cơ bản đã cài đặt đúng thuật toán Euclid để tìm UCLN (recursive). Tuy nhiên, có lỗi biên dịch do thiếu thư viện `iostream` cần thiết để sử dụng `std::cout` và `std::endl`.  Đây không phải là lỗi logic trong thuật toán, mà là lỗi cú pháp.  Thuật toán Euclid đệ quy hoạt động như sau:  nó dựa trên nguyên lý rằng UCLN(a, b) = UCLN(b, a % b), và khi b = 0 thì UCLN là a.  Hàm `timUCLN` đã thực hiện đúng điều này.
+Đoạn code của sinh viên sử dụng đệ quy để tìm UCLN bằng thuật toán Euclid, về cơ bản thuật toán là đúng. Tuy nhiên, đoạn code có lỗi biên dịch nghiêm trọng do thiếu khai báo thư viện `&lt;iostream&gt;` cần thiết để sử dụng `std::cout` và `std::endl`.  Đây không phải là lỗi logic trong thuật toán Euclid, mà là lỗi cú pháp.  Nếu bỏ qua lỗi biên dịch, thuật toán Euclid được triển khai chính xác.  Việc thiếu khai báo thư viện không cho phép chương trình biên dịch thành công.
 2. **Đề Xuất Sửa Lỗi:**
 ```cpp
 #include &lt;iostream&gt;
@@ -844,7 +858,7 @@
 }
 ```
 3. **Đánh Giá Chung:**
-Thuật toán tìm UCLN là đúng, tuy nhiên sinh viên cần chú ý đến việc thêm các thư viện cần thiết để chương trình biên dịch và chạy được. Lỗi thiếu thư viện là lỗi cú pháp, không phải lỗi logic.  Sinh viên cần cẩn thận hơn trong việc kiểm tra lỗi biên dịch.</t>
+Thuật toán tìm UCLN bằng đệ quy là đúng. Tuy nhiên, sinh viên cần chú ý hơn đến việc khai báo thư viện cần thiết trong C++.  Lỗi biên dịch khiến chương trình không thể chạy được.  Sinh viên cần xem lại các kiến thức cơ bản về cú pháp và việc sử dụng thư viện trong C++.</t>
         </is>
       </c>
     </row>

</xml_diff>